<commit_message>
update school code to Reframework
</commit_message>
<xml_diff>
--- a/botsDNA/SchoolInfo/Data/Config.xlsx
+++ b/botsDNA/SchoolInfo/Data/Config.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Personal\Uipath\botsDNA_SchoolUsecase\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Personal\Uipath\botsDNA\SchoolInfo\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56DD2CFB-18BB-4A4B-969F-A369DF8B654A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B15B72C9-DA50-405D-86BA-D9A05A8971CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="50">
   <si>
     <t>Name</t>
   </si>
@@ -163,6 +163,18 @@
   </si>
   <si>
     <t>SchoolUrl</t>
+  </si>
+  <si>
+    <t>outputFilePath</t>
+  </si>
+  <si>
+    <t>Data\Output\finalresult.xlsx</t>
+  </si>
+  <si>
+    <t>inputFilePath</t>
+  </si>
+  <si>
+    <t>Data\Input\MasterTemplate.xlsx</t>
   </si>
 </sst>
 </file>
@@ -548,7 +560,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -626,8 +638,22 @@
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" t="s">
+        <v>49</v>
+      </c>
+    </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>